<commit_message>
Updated Styles, Fixed Template Download
</commit_message>
<xml_diff>
--- a/Goodwill_schedule.xlsx
+++ b/Goodwill_schedule.xlsx
@@ -378,13 +378,13 @@
   </sheetPr>
   <dimension ref="A1:AS46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.2295918367347"/>
     <col collapsed="false" hidden="false" max="26" min="2" style="1" width="6.0765306122449"/>
     <col collapsed="false" hidden="true" max="27" min="27" style="1" width="0"/>
     <col collapsed="false" hidden="false" max="1025" min="28" style="1" width="6.0765306122449"/>

</xml_diff>